<commit_message>
feature drift - n0
</commit_message>
<xml_diff>
--- a/notebooks/Book1.xlsx
+++ b/notebooks/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="12671" windowHeight="9120" activeTab="1"/>
+    <workbookView windowWidth="22188" windowHeight="9120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="102">
   <si>
     <t>n0</t>
   </si>
@@ -181,24 +181,84 @@
     <t>c9</t>
   </si>
   <si>
+    <t>Linear increment to ~0.7</t>
+  </si>
+  <si>
     <t>Linear increment to 0.8</t>
   </si>
   <si>
+    <t>Linear increment to 0.2</t>
+  </si>
+  <si>
+    <t>Linear increment to ~0.45</t>
+  </si>
+  <si>
+    <t>Linear increment to ~0.35</t>
+  </si>
+  <si>
     <t>Gradual increment to -5</t>
   </si>
   <si>
     <t>Linear increment to - 0.8</t>
   </si>
   <si>
+    <t>~0.35</t>
+  </si>
+  <si>
+    <t>Gradual increment to 0.1</t>
+  </si>
+  <si>
+    <t>Linear Increment to ~ 0.4</t>
+  </si>
+  <si>
+    <t>Gradual increment to 0.2</t>
+  </si>
+  <si>
+    <t>Gradual increment to 0.8</t>
+  </si>
+  <si>
+    <t>Gradual Increment to 0.75</t>
+  </si>
+  <si>
+    <t>Gradual increment to 0.5</t>
+  </si>
+  <si>
     <t>Gradual increment to 3</t>
   </si>
   <si>
-    <t>Gradual increment to 0.8</t>
+    <t>Gradual Increment to ~0.55</t>
   </si>
   <si>
     <t>Suddent drift to 0</t>
   </si>
   <si>
+    <t>~0.55</t>
+  </si>
+  <si>
+    <t>Suddent drift to 0.8</t>
+  </si>
+  <si>
+    <t>Suddent drift to 0.6</t>
+  </si>
+  <si>
+    <t>Sudden drift to 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?Drift to 0.5 </t>
+  </si>
+  <si>
+    <t>Suddent drift to 0.5</t>
+  </si>
+  <si>
+    <t>?Drift to 0.5</t>
+  </si>
+  <si>
+    <t>Sudent drift</t>
+  </si>
+  <si>
+    <t>Suddent drift</t>
+  </si>
+  <si>
     <t>0 - 999</t>
   </si>
   <si>
@@ -224,9 +284,6 @@
   </si>
   <si>
     <t>5000 - 5999</t>
-  </si>
-  <si>
-    <t>Gradual increment to 0.2</t>
   </si>
   <si>
     <t>6000 - 6999</t>
@@ -470,7 +527,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,6 +573,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCEB4E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -987,7 +1062,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1011,16 +1086,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1029,89 +1104,89 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1133,15 +1208,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1158,16 +1224,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1175,8 +1232,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1193,6 +1250,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1202,37 +1262,55 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
@@ -1256,10 +1334,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1271,19 +1349,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1555,8 +1627,9 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="00FDFF6D"/>
       <color rgb="00FFFFCD"/>
-      <color rgb="00FDFF6D"/>
+      <color rgb="00CEB4E6"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1835,423 +1908,423 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="8.88888888888889" style="41"/>
-    <col min="9" max="9" width="8.88888888888889" style="41"/>
-    <col min="13" max="13" width="8.88888888888889" style="41"/>
-    <col min="17" max="17" width="8.88888888888889" style="41"/>
-    <col min="21" max="21" width="8.88888888888889" style="41"/>
+    <col min="5" max="5" width="8.88888888888889" style="42"/>
+    <col min="9" max="9" width="8.88888888888889" style="42"/>
+    <col min="13" max="13" width="8.88888888888889" style="42"/>
+    <col min="17" max="17" width="8.88888888888889" style="42"/>
+    <col min="21" max="21" width="8.88888888888889" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" s="38" customFormat="1" ht="19.95" spans="1:21">
-      <c r="A1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="43" t="s">
+    <row r="1" s="40" customFormat="1" ht="19.95" spans="1:21">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="44" t="s">
         <v>4</v>
       </c>
       <c r="U1" s="55"/>
     </row>
     <row r="3" ht="19.2" spans="1:17">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="45" t="s">
+      <c r="Q3" s="46" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A4" s="46" t="s">
+    <row r="4" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="47" t="s">
+      <c r="M4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="47" t="s">
+      <c r="Q4" s="48" t="s">
         <v>6</v>
       </c>
       <c r="U4" s="56"/>
     </row>
     <row r="5" ht="19.2" spans="1:17">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="45" t="s">
+      <c r="Q5" s="46" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A6" s="48" t="s">
+    <row r="6" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A6" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="E6" s="49" t="s">
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="E6" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="I6" s="47" t="s">
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="I6" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="49" t="s">
+      <c r="M6" s="50" t="s">
         <v>11</v>
       </c>
       <c r="N6" s="54"/>
       <c r="O6" s="54"/>
-      <c r="Q6" s="47" t="s">
+      <c r="Q6" s="48" t="s">
         <v>10</v>
       </c>
       <c r="U6" s="56"/>
     </row>
     <row r="7" ht="19.2" spans="1:17">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="45" t="s">
+      <c r="I7" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="45" t="s">
+      <c r="M7" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="45" t="s">
+      <c r="Q7" s="46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A8" s="46" t="s">
+    <row r="8" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A8" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="47" t="s">
+      <c r="M8" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="Q8" s="47" t="s">
+      <c r="Q8" s="48" t="s">
         <v>10</v>
       </c>
       <c r="U8" s="56"/>
     </row>
     <row r="9" ht="19.2" spans="1:17">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="I9" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="Q9" s="45" t="s">
+      <c r="Q9" s="46" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A10" s="46" t="s">
+    <row r="10" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A10" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="47" t="s">
+      <c r="I10" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="47" t="s">
+      <c r="M10" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="Q10" s="47" t="s">
+      <c r="Q10" s="48" t="s">
         <v>18</v>
       </c>
       <c r="U10" s="56"/>
     </row>
     <row r="11" ht="19.2" spans="1:17">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="45" t="s">
+      <c r="I11" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="45" t="s">
+      <c r="M11" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="45" t="s">
+      <c r="Q11" s="46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A12" s="46" t="s">
+    <row r="12" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A12" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="47" t="s">
+      <c r="I12" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="47" t="s">
+      <c r="M12" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="Q12" s="47" t="s">
+      <c r="Q12" s="48" t="s">
         <v>24</v>
       </c>
       <c r="U12" s="56"/>
     </row>
     <row r="13" ht="19.2" spans="1:17">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="45" t="s">
+      <c r="I13" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="M13" s="45" t="s">
+      <c r="M13" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="Q13" s="45" t="s">
+      <c r="Q13" s="46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A14" s="46" t="s">
+    <row r="14" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A14" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="47" t="s">
+      <c r="M14" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="Q14" s="47" t="s">
+      <c r="Q14" s="48" t="s">
         <v>24</v>
       </c>
       <c r="U14" s="56"/>
     </row>
     <row r="15" ht="19.2" spans="1:17">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="45" t="s">
+      <c r="I15" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="M15" s="45" t="s">
+      <c r="M15" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="45" t="s">
+      <c r="Q15" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A16" s="46" t="s">
+    <row r="16" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A16" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="47" t="s">
+      <c r="I16" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="M16" s="47" t="s">
+      <c r="M16" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="Q16" s="47" t="s">
+      <c r="Q16" s="48" t="s">
         <v>29</v>
       </c>
       <c r="U16" s="56"/>
     </row>
     <row r="17" ht="19.2" spans="1:17">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="45" t="s">
+      <c r="I17" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="45" t="s">
+      <c r="M17" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="Q17" s="45" t="s">
+      <c r="Q17" s="46" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A18" s="46" t="s">
+    <row r="18" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A18" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="47" t="s">
+      <c r="I18" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="47" t="s">
+      <c r="M18" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="Q18" s="47" t="s">
+      <c r="Q18" s="48" t="s">
         <v>32</v>
       </c>
       <c r="U18" s="56"/>
     </row>
     <row r="19" ht="19.2" spans="1:17">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="45" t="s">
+      <c r="E19" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="45" t="s">
+      <c r="I19" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="45" t="s">
+      <c r="M19" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="Q19" s="45" t="s">
+      <c r="Q19" s="46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A20" s="46" t="s">
+    <row r="20" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A20" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I20" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="47" t="s">
+      <c r="M20" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="Q20" s="47" t="s">
+      <c r="Q20" s="48" t="s">
         <v>32</v>
       </c>
       <c r="U20" s="56"/>
     </row>
     <row r="21" ht="19.2" spans="1:17">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="45" t="s">
+      <c r="E21" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="I21" s="45" t="s">
+      <c r="I21" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="M21" s="45" t="s">
+      <c r="M21" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="Q21" s="45" t="s">
+      <c r="Q21" s="46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" s="39" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A22" s="46" t="s">
+    <row r="22" s="41" customFormat="1" ht="19.2" spans="1:21">
+      <c r="A22" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="47" t="s">
+      <c r="I22" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="47" t="s">
+      <c r="M22" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="Q22" s="47" t="s">
+      <c r="Q22" s="48" t="s">
         <v>35</v>
       </c>
       <c r="U22" s="56"/>
     </row>
     <row r="23" ht="19.2" spans="1:17">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="45" t="s">
+      <c r="I23" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="M23" s="45" t="s">
+      <c r="M23" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="Q23" s="45" t="s">
+      <c r="Q23" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" ht="19.2" spans="1:17">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="51" t="s">
+      <c r="E24" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="51" t="s">
+      <c r="I24" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="M24" s="51" t="s">
+      <c r="M24" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="Q24" s="51" t="s">
+      <c r="Q24" s="52" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" s="40" customFormat="1" ht="19.2" spans="1:21">
-      <c r="A25" s="52" t="s">
+    <row r="25" s="8" customFormat="1" ht="19.2" spans="1:17">
+      <c r="A25" s="53" t="s">
         <v>38</v>
       </c>
       <c r="E25" s="53" t="s">
@@ -2266,56 +2339,55 @@
       <c r="Q25" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="U25" s="57"/>
     </row>
     <row r="26" ht="19.2" spans="1:17">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="51" t="s">
+      <c r="E26" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="51" t="s">
+      <c r="I26" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="M26" s="51" t="s">
+      <c r="M26" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="Q26" s="51" t="s">
+      <c r="Q26" s="52" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" ht="19.2" spans="1:17">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="45" t="s">
+      <c r="E27" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="45" t="s">
+      <c r="I27" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="M27" s="45" t="s">
+      <c r="M27" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="Q27" s="45" t="s">
+      <c r="Q27" s="46" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" ht="19.2" spans="1:17">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="51" t="s">
+      <c r="E28" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="51" t="s">
+      <c r="I28" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="M28" s="51" t="s">
+      <c r="M28" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="Q28" s="51" t="s">
+      <c r="Q28" s="52" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2339,75 +2411,80 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.22222222222222" style="12" customWidth="1"/>
-    <col min="2" max="2" width="8.88888888888889" style="12"/>
-    <col min="3" max="3" width="16.1111111111111" style="13" customWidth="1"/>
-    <col min="4" max="4" width="16.7777777777778" style="13" customWidth="1"/>
-    <col min="5" max="5" width="17" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.8888888888889" style="13" customWidth="1"/>
-    <col min="7" max="7" width="16.6666666666667" style="13" customWidth="1"/>
+    <col min="1" max="1" width="8.22222222222222" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.88888888888889" style="9"/>
+    <col min="3" max="3" width="16.1111111111111" style="10" customWidth="1"/>
+    <col min="4" max="4" width="16.7777777777778" style="10" customWidth="1"/>
+    <col min="5" max="5" width="17" style="10" customWidth="1"/>
+    <col min="6" max="6" width="15.8888888888889" style="10" customWidth="1"/>
+    <col min="7" max="7" width="16.6666666666667" style="10" customWidth="1"/>
+    <col min="8" max="8" width="17.037037037037" style="10" customWidth="1"/>
+    <col min="9" max="9" width="16.9074074074074" style="10" customWidth="1"/>
+    <col min="10" max="10" width="16.787037037037" style="10" customWidth="1"/>
+    <col min="11" max="11" width="16.4166666666667" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.3981481481481" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-    </row>
-    <row r="2" s="10" customFormat="1" spans="1:19">
-      <c r="A2" s="19" t="s">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" s="7" customFormat="1" spans="1:19">
+      <c r="A2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="15" t="s">
         <v>49</v>
       </c>
       <c r="M2" s="37"/>
@@ -2418,316 +2495,516 @@
       <c r="R2" s="37"/>
       <c r="S2" s="37"/>
     </row>
-    <row r="3" s="11" customFormat="1" spans="1:7">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-    </row>
-    <row r="4" ht="16.8" spans="1:7">
-      <c r="A4" s="25">
-        <v>0</v>
-      </c>
-      <c r="B4" s="25">
+    <row r="3" s="8" customFormat="1" spans="1:12">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" ht="16.8" spans="1:12">
+      <c r="A4" s="19">
+        <v>0</v>
+      </c>
+      <c r="B4" s="19">
         <v>999</v>
       </c>
-      <c r="C4" s="26">
-        <v>0</v>
-      </c>
-      <c r="D4" s="26">
-        <v>0</v>
-      </c>
-      <c r="E4" s="26">
-        <v>0</v>
-      </c>
-      <c r="F4" s="26">
-        <v>0</v>
-      </c>
-      <c r="G4" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" ht="33.6" spans="1:7">
-      <c r="A5" s="25">
+      <c r="C4" s="20">
+        <v>0</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0</v>
+      </c>
+      <c r="F4" s="20">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20">
+        <v>0</v>
+      </c>
+      <c r="H4" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" ht="33.6" spans="1:12">
+      <c r="A5" s="19">
         <v>1000</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="19">
         <v>1999</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="26">
-        <v>0</v>
-      </c>
-      <c r="F5" s="28" t="s">
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" ht="16.8" spans="1:7">
-      <c r="A6" s="25">
+      <c r="G5" s="20">
+        <v>0</v>
+      </c>
+      <c r="H5" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" ht="28.8" spans="1:12">
+      <c r="A6" s="19">
         <v>2000</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="19">
         <v>2999</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="24">
         <v>2</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="20">
         <v>1</v>
       </c>
-      <c r="E6" s="26">
-        <v>0</v>
-      </c>
-      <c r="F6" s="26">
+      <c r="E6" s="20">
+        <v>0</v>
+      </c>
+      <c r="F6" s="20">
         <v>-1</v>
       </c>
-      <c r="G6" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="33.6" spans="1:7">
-      <c r="A7" s="25">
+      <c r="G6" s="20">
+        <v>0</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" ht="33.6" spans="1:12">
+      <c r="A7" s="19">
         <v>3000</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="19">
         <v>3999</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="24">
         <v>2</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="20">
         <v>1</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="20">
         <v>-1</v>
       </c>
-      <c r="G7" s="28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" ht="33.6" spans="1:7">
-      <c r="A8" s="25">
+      <c r="G7" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" ht="33.6" spans="1:12">
+      <c r="A8" s="19">
         <v>4000</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="19">
         <v>4999</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="31" t="s">
+      <c r="E8" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" ht="16.8" spans="1:7">
-      <c r="A9" s="25">
+      <c r="G8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="I8" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" ht="28.8" spans="1:12">
+      <c r="A9" s="19">
         <v>5000</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="19">
         <v>5999</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="24">
         <v>-2</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="20">
         <v>-1</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="20">
         <v>-5</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="20">
         <v>1</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="20">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="10" ht="33.6" spans="1:7">
-      <c r="A10" s="25">
+      <c r="H9" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" ht="36" customHeight="1" spans="1:12">
+      <c r="A10" s="19">
         <v>6000</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="19">
         <v>6999</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="24">
         <v>-2</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="20">
         <v>-1</v>
       </c>
-      <c r="E10" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="26">
+      <c r="E10" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="20">
         <v>1</v>
       </c>
-      <c r="G10" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" ht="33.6" spans="1:7">
-      <c r="A11" s="25">
+      <c r="G10" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" ht="33.6" spans="1:12">
+      <c r="A11" s="19">
         <v>7000</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="19">
         <v>7999</v>
       </c>
-      <c r="C11" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" ht="16.8" spans="1:7">
-      <c r="A12" s="25">
+      <c r="C11" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" ht="28.8" spans="1:12">
+      <c r="A12" s="19">
         <v>8000</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="19">
         <v>8999</v>
       </c>
-      <c r="C12" s="29">
-        <v>0</v>
-      </c>
-      <c r="D12" s="26">
-        <v>0</v>
-      </c>
-      <c r="E12" s="26">
-        <v>0</v>
-      </c>
-      <c r="F12" s="26">
-        <v>0</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" ht="16.8" spans="1:7">
-      <c r="A13" s="25">
+      <c r="C12" s="24">
+        <v>0</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
+        <v>0</v>
+      </c>
+      <c r="G12" s="20">
+        <v>0</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" ht="16.8" spans="1:12">
+      <c r="A13" s="19">
         <v>9000</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="19">
         <v>9999</v>
       </c>
-      <c r="C13" s="29">
-        <v>0</v>
-      </c>
-      <c r="D13" s="26">
-        <v>0</v>
-      </c>
-      <c r="E13" s="34">
-        <v>0</v>
-      </c>
-      <c r="F13" s="26">
-        <v>0</v>
-      </c>
-      <c r="G13" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" ht="16.8" spans="1:7">
-      <c r="A14" s="25">
+      <c r="C13" s="24">
+        <v>0</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0</v>
+      </c>
+      <c r="E13" s="32">
+        <v>0</v>
+      </c>
+      <c r="F13" s="20">
+        <v>0</v>
+      </c>
+      <c r="G13" s="32">
+        <v>0</v>
+      </c>
+      <c r="H13" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" ht="16.8" spans="1:12">
+      <c r="A14" s="33">
         <v>10000</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="33">
         <v>10999</v>
       </c>
-      <c r="C14" s="29">
-        <v>0</v>
-      </c>
-      <c r="D14" s="26">
-        <v>0</v>
-      </c>
-      <c r="E14" s="26">
-        <v>0</v>
-      </c>
-      <c r="F14" s="26">
-        <v>0</v>
-      </c>
-      <c r="G14" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" ht="16.8" spans="1:7">
-      <c r="A15" s="25">
+      <c r="C14" s="34">
+        <v>0</v>
+      </c>
+      <c r="D14" s="35">
+        <v>0</v>
+      </c>
+      <c r="E14" s="35">
+        <v>0</v>
+      </c>
+      <c r="F14" s="35">
+        <v>0</v>
+      </c>
+      <c r="G14" s="35">
+        <v>0</v>
+      </c>
+      <c r="H14" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="L14" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" ht="16.8" spans="1:12">
+      <c r="A15" s="33">
         <v>11000</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="33">
         <v>11999</v>
       </c>
-      <c r="C15" s="29">
-        <v>0</v>
-      </c>
-      <c r="D15" s="26">
-        <v>0</v>
-      </c>
-      <c r="E15" s="26">
-        <v>0</v>
-      </c>
-      <c r="F15" s="26">
-        <v>0</v>
-      </c>
-      <c r="G15" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" ht="16.8" spans="1:7">
-      <c r="A16" s="25">
+      <c r="C15" s="34">
+        <v>0</v>
+      </c>
+      <c r="D15" s="35">
+        <v>0</v>
+      </c>
+      <c r="E15" s="35">
+        <v>0</v>
+      </c>
+      <c r="F15" s="35">
+        <v>0</v>
+      </c>
+      <c r="G15" s="35">
+        <v>0</v>
+      </c>
+      <c r="H15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" ht="16.8" spans="1:12">
+      <c r="A16" s="33">
         <v>12000</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="33">
         <v>12999</v>
       </c>
-      <c r="C16" s="29">
-        <v>0</v>
-      </c>
-      <c r="D16" s="26">
-        <v>0</v>
-      </c>
-      <c r="E16" s="26">
-        <v>0</v>
-      </c>
-      <c r="F16" s="26">
-        <v>0</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
+      <c r="C16" s="34">
+        <v>0</v>
+      </c>
+      <c r="D16" s="35">
+        <v>0</v>
+      </c>
+      <c r="E16" s="35">
+        <v>0</v>
+      </c>
+      <c r="F16" s="35">
+        <v>0</v>
+      </c>
+      <c r="G16" s="35">
+        <v>0</v>
+      </c>
+      <c r="H16" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="36">
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="35"/>
+      <c r="B17" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2790,13 +3067,13 @@
       <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" ht="17.55" spans="1:11">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -2814,24 +3091,24 @@
         <v>0</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>57</v>
+        <v>77</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" ht="17.55" spans="1:11">
       <c r="A3" s="3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2849,24 +3126,24 @@
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>57</v>
+        <v>77</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" ht="17.55" spans="1:11">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
@@ -2884,24 +3161,24 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>57</v>
+        <v>77</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5" ht="17.55" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
@@ -2919,24 +3196,24 @@
         <v>18</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>61</v>
+        <v>77</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" ht="17.55" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>20</v>
@@ -2951,7 +3228,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G6" s="4">
         <v>0.8</v>
@@ -2965,13 +3242,13 @@
       <c r="J6" s="4">
         <v>-1</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" ht="17.55" spans="1:11">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4">
         <v>-2</v>
@@ -2986,13 +3263,13 @@
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="I7" s="4">
         <v>0.25</v>
@@ -3000,13 +3277,13 @@
       <c r="J7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="8" ht="17.55" spans="1:11">
       <c r="A8" s="3" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B8" s="4">
         <v>-2</v>
@@ -3030,18 +3307,18 @@
         <v>0.8</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="J8" s="4">
         <v>1</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>68</v>
+      <c r="K8" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" ht="17.55" spans="1:11">
       <c r="A9" s="3" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -3056,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="G9" s="4">
         <v>0.2</v>
@@ -3070,13 +3347,13 @@
       <c r="J9" s="4">
         <v>1</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" ht="17.55" spans="1:11">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
@@ -3091,7 +3368,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="G10" s="4">
         <v>0.5</v>
@@ -3105,13 +3382,13 @@
       <c r="J10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" ht="17.55" spans="1:11">
       <c r="A11" s="3" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B11" s="4">
         <v>0</v>
@@ -3140,13 +3417,13 @@
       <c r="J11" s="4">
         <v>0</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="4">
         <v>0.125</v>
       </c>
     </row>
     <row r="12" ht="17.55" spans="1:11">
       <c r="A12" s="3" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -3161,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="G12" s="4">
         <v>0.5</v>
@@ -3170,18 +3447,18 @@
         <v>0.5</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="J12" s="4">
         <v>0</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>76</v>
+      <c r="K12" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" ht="17.55" spans="1:11">
       <c r="A13" s="3" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -3196,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="G13" s="4">
         <v>0.5</v>
@@ -3205,18 +3482,18 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="J13" s="4">
         <v>0</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>79</v>
+      <c r="K13" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" ht="16.8" spans="1:11">
       <c r="A14" s="5" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
@@ -3231,7 +3508,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="G14" s="6">
         <v>0.5</v>
@@ -3240,13 +3517,13 @@
         <v>0.5</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="J14" s="6">
         <v>0</v>
       </c>
-      <c r="K14" s="9" t="s">
-        <v>82</v>
+      <c r="K14" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>